<commit_message>
test edit doc et excel
</commit_message>
<xml_diff>
--- a/pc/Periode de test 3 semaines.xlsx
+++ b/pc/Periode de test 3 semaines.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\promo\052021\pro\data\pc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27379B13-A2CE-4C3B-9F73-12AC73811CE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="576" yWindow="60" windowWidth="18792" windowHeight="8844" tabRatio="588"/>
+    <workbookView xWindow="-48" yWindow="-48" windowWidth="23136" windowHeight="12336" tabRatio="588" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -15,8 +21,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Djamel MOUCHENE</author>
+  </authors>
+  <commentList>
+    <comment ref="R7" authorId="0" shapeId="0" xr:uid="{5CB0BF0F-142D-4626-AA50-A90567FDFC2B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Djamel MOUCHENE:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+En fait bonsoir !!! ;)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>Semaine 1</t>
   </si>
@@ -207,13 +247,22 @@
   <si>
     <t xml:space="preserve">Enquête de 
 satisfaction </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonjour </t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>alpha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +294,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -878,6 +940,63 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -905,9 +1024,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -928,60 +1044,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -992,6 +1054,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1040,7 +1105,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1073,9 +1138,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1108,6 +1190,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1283,11 +1382,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1314,65 +1413,65 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="47"/>
-      <c r="B2" s="71" t="s">
+      <c r="A2" s="66"/>
+      <c r="B2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="74" t="s">
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="71" t="s">
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="72"/>
-      <c r="P2" s="72"/>
-      <c r="Q2" s="72"/>
-      <c r="R2" s="73"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
+      <c r="Q2" s="56"/>
+      <c r="R2" s="57"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="47"/>
-      <c r="B3" s="65" t="s">
+      <c r="A3" s="66"/>
+      <c r="B3" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="65" t="s">
+      <c r="C3" s="54"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="66"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="79" t="s">
+      <c r="F3" s="50"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="80"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="79" t="s">
+      <c r="I3" s="64"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="81"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="65" t="s">
+      <c r="L3" s="65"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="70"/>
-      <c r="P3" s="66"/>
-      <c r="Q3" s="65" t="s">
+      <c r="O3" s="54"/>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="R3" s="66"/>
+      <c r="R3" s="50"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="47"/>
+      <c r="A4" s="66"/>
       <c r="B4" s="15" t="s">
         <v>43</v>
       </c>
@@ -1384,7 +1483,7 @@
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="17"/>
-      <c r="G4" s="68"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="18" t="s">
         <v>46</v>
       </c>
@@ -1396,7 +1495,7 @@
       </c>
       <c r="K4" s="18"/>
       <c r="L4" s="20"/>
-      <c r="M4" s="77"/>
+      <c r="M4" s="61"/>
       <c r="N4" s="15" t="s">
         <v>44</v>
       </c>
@@ -1410,7 +1509,7 @@
       <c r="R4" s="17"/>
     </row>
     <row r="5" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="47"/>
+      <c r="A5" s="66"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1426,7 +1525,7 @@
       <c r="F5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="68"/>
+      <c r="G5" s="52"/>
       <c r="H5" s="6" t="s">
         <v>8</v>
       </c>
@@ -1442,7 +1541,7 @@
       <c r="L5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="77"/>
+      <c r="M5" s="61"/>
       <c r="N5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1466,60 +1565,62 @@
       <c r="B6" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="C6" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="50" t="s">
+      <c r="D6" s="69" t="s">
         <v>58</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="23"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="56" t="s">
+      <c r="G6" s="52"/>
+      <c r="H6" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="53" t="s">
+      <c r="I6" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="50" t="s">
+      <c r="J6" s="69" t="s">
         <v>51</v>
       </c>
       <c r="K6" s="24"/>
       <c r="L6" s="25"/>
-      <c r="M6" s="77"/>
-      <c r="N6" s="56" t="s">
+      <c r="M6" s="61"/>
+      <c r="N6" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="O6" s="53" t="s">
+      <c r="O6" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="P6" s="50" t="s">
+      <c r="P6" s="69" t="s">
         <v>53</v>
       </c>
       <c r="Q6" s="26"/>
-      <c r="R6" s="27"/>
+      <c r="R6" s="27" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="7" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="62"/>
-      <c r="D7" s="51"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="70"/>
       <c r="E7" s="22"/>
       <c r="F7" s="23"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="51"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="70"/>
       <c r="K7" s="24"/>
       <c r="L7" s="25"/>
-      <c r="M7" s="77"/>
-      <c r="N7" s="57"/>
-      <c r="O7" s="54"/>
-      <c r="P7" s="51"/>
+      <c r="M7" s="61"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="70"/>
       <c r="Q7" s="26"/>
       <c r="R7" s="27"/>
     </row>
@@ -1527,21 +1628,21 @@
       <c r="A8" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="49"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="52"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="71"/>
       <c r="E8" s="22"/>
       <c r="F8" s="23"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="71"/>
       <c r="K8" s="24"/>
       <c r="L8" s="25"/>
-      <c r="M8" s="77"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="55"/>
-      <c r="P8" s="52"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="76"/>
+      <c r="O8" s="74"/>
+      <c r="P8" s="71"/>
       <c r="Q8" s="26"/>
       <c r="R8" s="27"/>
     </row>
@@ -1554,13 +1655,13 @@
       <c r="D9" s="30"/>
       <c r="E9" s="31"/>
       <c r="F9" s="30"/>
-      <c r="G9" s="68"/>
+      <c r="G9" s="52"/>
       <c r="H9" s="31"/>
       <c r="I9" s="29"/>
       <c r="J9" s="30"/>
       <c r="K9" s="31"/>
       <c r="L9" s="30"/>
-      <c r="M9" s="77"/>
+      <c r="M9" s="61"/>
       <c r="N9" s="32"/>
       <c r="O9" s="33"/>
       <c r="P9" s="34"/>
@@ -1571,10 +1672,10 @@
       <c r="A10" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="72" t="s">
         <v>56</v>
       </c>
       <c r="D10" s="35" t="s">
@@ -1582,19 +1683,19 @@
       </c>
       <c r="E10" s="26"/>
       <c r="F10" s="27"/>
-      <c r="G10" s="68"/>
+      <c r="G10" s="52"/>
       <c r="H10" s="36" t="s">
         <v>26</v>
       </c>
       <c r="I10" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="50" t="s">
+      <c r="J10" s="69" t="s">
         <v>30</v>
       </c>
       <c r="K10" s="26"/>
       <c r="L10" s="27"/>
-      <c r="M10" s="77"/>
+      <c r="M10" s="61"/>
       <c r="N10" s="36" t="s">
         <v>32</v>
       </c>
@@ -1611,27 +1712,27 @@
       <c r="A11" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="49"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="50" t="s">
+      <c r="B11" s="68"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="69" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="26"/>
       <c r="F11" s="27"/>
-      <c r="G11" s="68"/>
+      <c r="G11" s="52"/>
       <c r="H11" s="36" t="s">
         <v>34</v>
       </c>
       <c r="I11" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="51"/>
+      <c r="J11" s="70"/>
       <c r="K11" s="26"/>
       <c r="L11" s="27"/>
-      <c r="M11" s="77"/>
+      <c r="M11" s="61"/>
       <c r="N11" s="36"/>
       <c r="O11" s="37"/>
-      <c r="P11" s="53" t="s">
+      <c r="P11" s="72" t="s">
         <v>52</v>
       </c>
       <c r="Q11" s="38"/>
@@ -1644,26 +1745,26 @@
       <c r="B12" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="72" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="51"/>
+      <c r="D12" s="70"/>
       <c r="E12" s="26"/>
       <c r="F12" s="27"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="56" t="s">
+      <c r="G12" s="52"/>
+      <c r="H12" s="47" t="s">
         <v>27</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="51"/>
+      <c r="J12" s="70"/>
       <c r="K12" s="26"/>
       <c r="L12" s="27"/>
-      <c r="M12" s="77"/>
+      <c r="M12" s="61"/>
       <c r="N12" s="36"/>
       <c r="O12" s="37"/>
-      <c r="P12" s="54"/>
+      <c r="P12" s="73"/>
       <c r="Q12" s="38"/>
       <c r="R12" s="27"/>
     </row>
@@ -1672,39 +1773,27 @@
         <v>42</v>
       </c>
       <c r="B13" s="40"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="59"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="77"/>
       <c r="E13" s="41"/>
       <c r="F13" s="42"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="64"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="48"/>
       <c r="I13" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="J13" s="59"/>
+      <c r="J13" s="77"/>
       <c r="K13" s="41"/>
       <c r="L13" s="42"/>
-      <c r="M13" s="78"/>
+      <c r="M13" s="62"/>
       <c r="N13" s="44"/>
       <c r="O13" s="45"/>
-      <c r="P13" s="55"/>
+      <c r="P13" s="74"/>
       <c r="Q13" s="46"/>
       <c r="R13" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="G2:G13"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="M2:M13"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="N3:P3"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="J6:J8"/>
@@ -1721,14 +1810,27 @@
     <mergeCell ref="D11:D13"/>
     <mergeCell ref="H6:H8"/>
     <mergeCell ref="I6:I8"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="G2:G13"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="M2:M13"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="N3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1740,13 +1842,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>